<commit_message>
Updated the amount of hours. I forgot to do it the 25.
</commit_message>
<xml_diff>
--- a/deliveries/AmountOfHours_MeteoCal_MGFFJJ.xlsx
+++ b/deliveries/AmountOfHours_MeteoCal_MGFFJJ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\AppData\Local\Temp\deliveries.svn000.tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="B1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,9 +523,15 @@
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C8" s="1">
+        <v>165</v>
+      </c>
+      <c r="D8" s="1">
+        <v>205</v>
+      </c>
+      <c r="E8" s="1">
+        <v>70</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -554,15 +560,15 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C6:C10)</f>
-        <v>111</v>
+        <v>276</v>
       </c>
       <c r="D12" s="6">
         <f>SUM(D6:D10)</f>
-        <v>137</v>
+        <v>342</v>
       </c>
       <c r="E12" s="6">
         <f>SUM(E6:E10)</f>
-        <v>69</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -575,18 +581,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,6 +736,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52A29D2-922D-49A6-A334-36D6FDA90E27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20E6988C-4DA7-4CEA-8D0C-AAE2BA779028}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -741,14 +755,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52A29D2-922D-49A6-A334-36D6FDA90E27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>